<commit_message>
Deleted files, minor updates
Deleted reference material and some other unnecessary material; Updates
to minor parts
</commit_message>
<xml_diff>
--- a/InventorModel/Extruder/SanladererBowdenExtruder/SanladererBowdenExtruder BOM.xlsx
+++ b/InventorModel/Extruder/SanladererBowdenExtruder/SanladererBowdenExtruder BOM.xlsx
@@ -31,7 +31,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Extruder\SanladererBowdenExtruder\SanladererBowdenArm.ipt</t>
+          <t>C:\Users\Jack\ownCloud\Projects\CrossBot\InventorModel\Extruder\SanladererBowdenExtruder\SanladererBowdenArm.ipt</t>
         </r>
       </text>
     </comment>
@@ -45,7 +45,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Extruder\SanladererBowdenExtruder\SanladererBowdenBody.ipt</t>
+          <t>C:\Users\Jack\ownCloud\Projects\CrossBot\InventorModel\Extruder\SanladererBowdenExtruder\SanladererBowdenBody.ipt</t>
         </r>
       </text>
     </comment>
@@ -59,7 +59,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Electronics\Motors\StepperMotorNema17.ipt</t>
+          <t>C:\Users\Jack\ownCloud\Projects\CrossBot\InventorModel\Electronics\Motors\StepperMotorNema17.ipt</t>
         </r>
       </text>
     </comment>
@@ -73,7 +73,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Hardware\Extruder\DriveGearMK8.ipt</t>
+          <t>C:\Users\Jack\ownCloud\Projects\CrossBot\InventorModel\Hardware\Extruder\DriveGearMK8.ipt</t>
         </r>
       </text>
     </comment>
@@ -87,7 +87,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Hardware\Bearing\BearingRadialBall\BearingRadialBall624zz.ipt</t>
+          <t>C:\Users\Jack\ownCloud\Projects\CrossBot\InventorModel\Hardware\Bearing\BearingRadialBall\BearingRadialBall624zz.ipt</t>
         </r>
       </text>
     </comment>
@@ -101,7 +101,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Hardware\Bolts\SHCS\SHCS3\SHCS3x18.ipt</t>
+          <t>C:\Users\Jack\ownCloud\Projects\CrossBot\InventorModel\Hardware\BoltWashers\BoltWasher3\BoltWasher3x18.iam</t>
         </r>
       </text>
     </comment>
@@ -115,7 +115,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Hardware\Wahsers\M3Washer.ipt</t>
+          <t>C:\Users\Jack\ownCloud\Projects\CrossBot\InventorModel\Hardware\BoltWashers\BoltWasher4\BoltWasher4x18.iam</t>
         </r>
       </text>
     </comment>
@@ -129,35 +129,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Hardware\Bolts\SHCS\SHCS4\SHCS4x18.ipt</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Hardware\Wahsers\M4Washer.ipt</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>C:\Users\Jack\ownCloud\Projects\CoreXY\InventorModel\Hardware\Bolts\SHCS\SHCS4\SHCS4x10.ipt</t>
+          <t>C:\Users\Jack\ownCloud\Projects\CrossBot\InventorModel\Hardware\BoltWashers\BoltWasher4\BoltWasher4x10.iam</t>
         </r>
       </text>
     </comment>
@@ -166,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>PART PREVIEW</t>
   </si>
@@ -186,9 +158,6 @@
     <t>TITLE</t>
   </si>
   <si>
-    <t>AUTHOR</t>
-  </si>
-  <si>
     <t>CATEGORY</t>
   </si>
   <si>
@@ -213,7 +182,10 @@
     <t>Sanladerer Bowden Arm</t>
   </si>
   <si>
-    <t>Jack</t>
+    <t>Print</t>
+  </si>
+  <si>
+    <t>This is a rework of Thomas Sanladerer's bowden extruder. The most notable change is that this version is significantly thinner than the original.</t>
   </si>
   <si>
     <t>Jack; Thomas Sanladerer</t>
@@ -231,6 +203,9 @@
     <t>NEMA 17 x 60(?) Stepper Motor</t>
   </si>
   <si>
+    <t>Electronics</t>
+  </si>
+  <si>
     <t>Misumi</t>
   </si>
   <si>
@@ -240,6 +215,9 @@
     <t>MK8 Drive Gear</t>
   </si>
   <si>
+    <t>Hardware</t>
+  </si>
+  <si>
     <t>RobotDigg</t>
   </si>
   <si>
@@ -252,61 +230,25 @@
     <t>http://us.misumi-ec.com/vona2/detail/110302273450</t>
   </si>
   <si>
-    <t>M3x18SHCS</t>
-  </si>
-  <si>
-    <t>SHCS 4x18</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>CB3-18</t>
-  </si>
-  <si>
-    <t>M3Washer</t>
-  </si>
-  <si>
-    <t>M3 Washer</t>
-  </si>
-  <si>
-    <t>PWF3</t>
-  </si>
-  <si>
-    <t>http://us.misumi-ec.com/vona2/detail/110300252910/</t>
-  </si>
-  <si>
-    <t>M4x18SHCS</t>
-  </si>
-  <si>
-    <t>CB4-18</t>
-  </si>
-  <si>
-    <t>M4Washer</t>
-  </si>
-  <si>
-    <t>M4 Washer</t>
-  </si>
-  <si>
-    <t>PWF4</t>
-  </si>
-  <si>
-    <t>M4x10SHCS</t>
-  </si>
-  <si>
-    <t>Frame Brace Screws</t>
-  </si>
-  <si>
-    <t>CB4-10</t>
-  </si>
-  <si>
-    <t>http://us.misumi-ec.com/vona2/detail/110300239070/</t>
+    <t>BoltWasher3x18</t>
+  </si>
+  <si>
+    <t>Bolt Washer 3x18</t>
+  </si>
+  <si>
+    <t>BoltWasher4x18</t>
+  </si>
+  <si>
+    <t>BoltWasher4x10</t>
+  </si>
+  <si>
+    <t>Bolt + Washer 3x24</t>
   </si>
   <si>
     <t xml:space="preserve">ASSEMBLY PARTS TOTAL = </t>
   </si>
   <si>
-    <t>File created: 2/2/2015 21:03:26</t>
+    <t>File created: 19/3/2015 8:38:04</t>
   </si>
 </sst>
 </file>
@@ -745,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,15 +701,14 @@
     <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="130.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,16 +742,13 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -823,22 +761,23 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -857,19 +796,20 @@
         <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>19</v>
@@ -888,22 +828,21 @@
         <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -916,25 +855,24 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -947,212 +885,114 @@
         <v>3.64</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="K6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3">
         <v>4</v>
       </c>
       <c r="D7" s="4">
-        <v>0.26</v>
+        <v>0.42</v>
       </c>
       <c r="E7" s="4">
         <f>SUM(C7*D7)</f>
-        <v>1.04</v>
+        <v>1.68</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>0.16</v>
+        <v>0.42</v>
       </c>
       <c r="E8" s="4">
         <f>SUM(C8*D8)</f>
-        <v>0.64</v>
-      </c>
-      <c r="F8" s="2" t="s">
+        <v>0.42</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="4">
-        <v>0.26</v>
+        <v>0.42</v>
       </c>
       <c r="E9" s="4">
         <f>SUM(C9*D9)</f>
-        <v>0.26</v>
+        <v>0.84</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.16</v>
-      </c>
-      <c r="E10" s="4">
-        <f>SUM(C10*D10)</f>
-        <v>0.48</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="2" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.26</v>
-      </c>
-      <c r="E11" s="4">
-        <f>SUM(C11*D11)</f>
-        <v>0.52</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="6">
-        <f>SUM(E2:E11)</f>
-        <v>6.5799999999999983</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
+      <c r="E10" s="6">
+        <f>SUM(E2:E9)</f>
+        <v>6.58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>